<commit_message>
add ruleName, question suffix
</commit_message>
<xml_diff>
--- a/TestProject/TestProject/wwwroot/upload/template_2016CSE.xlsx
+++ b/TestProject/TestProject/wwwroot/upload/template_2016CSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/GraduationAssessment/GraduationAssesment/TestProject/TestProject/wwwroot/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D38DC06-163B-2F44-BA75-18C2F0046CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A0BF68-1030-4245-807F-86836C6663C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,10 +144,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>평점평균 기준을 입력하세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>평점평균</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -694,6 +690,10 @@
   </si>
   <si>
     <t>주니어디자인프로젝트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점평균 기준을 입력하세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1266,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1283,22 +1283,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1312,10 +1312,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="48">
@@ -1326,10 +1326,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1337,13 +1337,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" t="s">
         <v>42</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1357,7 +1357,7 @@
         <v>2016</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1371,7 +1371,7 @@
         <v>2016</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1385,16 +1385,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1402,16 +1402,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1428,7 +1428,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1439,13 +1439,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1456,13 +1456,13 @@
         <v>10</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1470,7 +1470,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="17">
         <v>4</v>
@@ -1479,7 +1479,7 @@
         <v>25</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1490,13 +1490,13 @@
         <v>11</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1507,13 +1507,13 @@
         <v>12</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1521,7 +1521,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="17">
         <v>0</v>
@@ -1530,10 +1530,10 @@
         <v>25</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1550,7 +1550,7 @@
         <v>25</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1564,13 +1564,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1587,7 +1587,7 @@
         <v>25</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1604,7 +1604,7 @@
         <v>25</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1615,13 +1615,13 @@
         <v>17</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1629,16 +1629,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1649,13 +1649,13 @@
         <v>18</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1672,7 +1672,7 @@
         <v>25</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1689,7 +1689,7 @@
         <v>25</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1700,16 +1700,16 @@
         <v>24</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1717,16 +1717,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1734,19 +1734,19 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="20">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1754,16 +1754,16 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="20">
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -1772,16 +1772,16 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1789,16 +1789,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1815,7 +1815,7 @@
         <v>25</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G31" t="s">
         <v>23</v>
@@ -1826,16 +1826,16 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="D32" s="20">
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
@@ -1843,22 +1843,22 @@
     </row>
     <row r="33" spans="1:7" ht="48">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4">
         <v>32</v>
       </c>
       <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>89</v>
-      </c>
       <c r="E33" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="48">
@@ -1866,16 +1866,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1883,16 +1883,16 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1900,7 +1900,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" s="20">
         <v>2</v>
@@ -1909,7 +1909,7 @@
         <v>25</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1917,19 +1917,19 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1937,7 +1937,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D38" s="20">
         <v>0</v>
@@ -1946,7 +1946,7 @@
         <v>25</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1954,19 +1954,19 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1974,19 +1974,19 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2013,33 +2013,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -2056,10 +2056,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -2186,33 +2186,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -2229,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3" s="27">
         <v>3</v>
@@ -2249,10 +2249,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>159</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>160</v>
       </c>
       <c r="D4" s="27">
         <v>3</v>
@@ -2371,21 +2371,21 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>63</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
       <c r="I1" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
@@ -2394,57 +2394,57 @@
     <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="28"/>
       <c r="B2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="E2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="G2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="I2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="K2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="D3" s="9">
         <v>2017</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="G3" s="9">
         <v>2012</v>
@@ -2651,21 +2651,21 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>63</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
       <c r="I1" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
@@ -2674,57 +2674,57 @@
     <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="28"/>
       <c r="B2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="E2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="G2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="I2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="K2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="D3" s="9">
         <v>2017</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" s="9">
         <v>2012</v>
@@ -2928,33 +2928,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -3088,30 +3088,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -3125,10 +3125,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -3142,10 +3142,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
@@ -3159,10 +3159,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
@@ -3176,10 +3176,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="5">
         <v>2</v>
@@ -3193,10 +3193,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="5">
         <v>3</v>
@@ -3210,10 +3210,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="5">
         <v>3</v>
@@ -3227,10 +3227,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="5">
         <v>3</v>
@@ -3289,30 +3289,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -3326,10 +3326,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -3343,10 +3343,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" s="5">
         <v>3</v>
@@ -3360,10 +3360,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D5" s="5">
         <v>3</v>
@@ -3377,10 +3377,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="5">
         <v>3</v>
@@ -3394,10 +3394,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="D7" s="5">
         <v>3</v>
@@ -3474,30 +3474,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -3511,10 +3511,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="23">
         <v>3</v>
@@ -3528,10 +3528,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="23">
         <v>3</v>
@@ -3545,10 +3545,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="23">
         <v>3</v>
@@ -3642,30 +3642,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -3679,10 +3679,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="23">
         <v>4</v>
@@ -3696,10 +3696,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" s="23">
         <v>4</v>
@@ -3713,10 +3713,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="23">
         <v>4</v>
@@ -3730,10 +3730,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" s="23">
         <v>4</v>
@@ -3747,10 +3747,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="23">
         <v>4</v>
@@ -3764,10 +3764,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D8" s="23">
         <v>4</v>
@@ -3834,30 +3834,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -3979,30 +3979,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -4126,33 +4126,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -4169,10 +4169,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -4189,10 +4189,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" s="5">
         <v>3</v>
@@ -4209,10 +4209,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5" s="5">
         <v>3</v>
@@ -4229,10 +4229,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="5">
         <v>3</v>
@@ -4328,33 +4328,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -4371,10 +4371,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>

</xml_diff>